<commit_message>
test data changes for PROD
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/openCartTestData.xlsx
+++ b/src/test/resources/testData/openCartTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\naveens\SelOpenCartPractise\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA92DC73-6650-450A-B767-5851D5C7F750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3B4240-7C8B-4BB4-BB91-3B6B4A98F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B7A9D1AA-D4D0-4F22-9549-24F180A9205D}"/>
   </bookViews>
@@ -84,13 +84,13 @@
     <t>harithaPROD</t>
   </si>
   <si>
-    <t>auto23manickam.6789@gmail.com</t>
-  </si>
-  <si>
-    <t>auto23monika.6789@gmail.com</t>
-  </si>
-  <si>
-    <t>auto23haritha.67889@gmail.com</t>
+    <t>auto99manickam.6789@gmail.com</t>
+  </si>
+  <si>
+    <t>auto99monika.6789@gmail.com</t>
+  </si>
+  <si>
+    <t>auto99haritha.67889@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
config test data changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/openCartTestData.xlsx
+++ b/src/test/resources/testData/openCartTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\naveens\SelOpenCartPractise\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D10A54-058D-4FE7-8354-023CFB65DB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D438A-AAEF-47FF-B775-1073CE70022E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B7A9D1AA-D4D0-4F22-9549-24F180A9205D}"/>
   </bookViews>
@@ -75,19 +75,19 @@
     <t>badhrachalam</t>
   </si>
   <si>
-    <t>auto99manickam.109@gmail.com</t>
-  </si>
-  <si>
-    <t>auto99monika.109@gmail.com</t>
-  </si>
-  <si>
-    <t>auto99haritha.109@gmail.com</t>
-  </si>
-  <si>
     <t>monika</t>
   </si>
   <si>
     <t>haritha</t>
+  </si>
+  <si>
+    <t>107automanickam@gmail.com</t>
+  </si>
+  <si>
+    <t>107automonika@gmail.com</t>
+  </si>
+  <si>
+    <t>107autoharitha@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,7 +501,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -515,13 +515,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -535,13 +535,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
random email ID changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/openCartTestData.xlsx
+++ b/src/test/resources/testData/openCartTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\naveens\SelOpenCartPractise\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC200487-C5A0-44F2-B634-1651A2A939D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7B4CA7-3089-4C50-8B07-A145DCBE7837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B7A9D1AA-D4D0-4F22-9549-24F180A9205D}"/>
   </bookViews>
@@ -81,13 +81,13 @@
     <t>haritha</t>
   </si>
   <si>
-    <t>109automanickam@gmail.com</t>
-  </si>
-  <si>
-    <t>109automonika@gmail.com</t>
-  </si>
-  <si>
-    <t>109autoharitha@gmail.com</t>
+    <t>AutomationManickam@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationMonika@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationHaritha@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>